<commit_message>
Análisis de casos de uso del sistema
</commit_message>
<xml_diff>
--- a/Cálculo duraciones PE.xlsx
+++ b/Cálculo duraciones PE.xlsx
@@ -403,7 +403,7 @@
   <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -568,7 +568,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -576,7 +576,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -584,7 +584,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -592,7 +592,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -600,7 +600,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -681,7 +681,7 @@
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <f>SUM(A20:A33)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B34" s="1">
         <f>SUM(B20:B33)</f>
@@ -905,7 +905,7 @@
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
         <f>SUM(A18,A34,A41,A51,A59)</f>
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B62">
         <f>SUM(B18,B34,B41,B51,B59)</f>

</xml_diff>

<commit_message>
Añadidas fotos de Casos de uso y de modelo de dominio
</commit_message>
<xml_diff>
--- a/Cálculo duraciones PE.xlsx
+++ b/Cálculo duraciones PE.xlsx
@@ -403,7 +403,7 @@
   <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -608,7 +608,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -616,7 +616,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -624,7 +624,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B27">
         <v>5</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B28">
         <v>2</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -681,7 +681,7 @@
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <f>SUM(A20:A33)</f>
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B34" s="1">
         <f>SUM(B20:B33)</f>
@@ -905,7 +905,7 @@
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
         <f>SUM(A18,A34,A41,A51,A59)</f>
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B62">
         <f>SUM(B18,B34,B41,B51,B59)</f>

</xml_diff>

<commit_message>
Finalizado Análisis del programa
</commit_message>
<xml_diff>
--- a/Cálculo duraciones PE.xlsx
+++ b/Cálculo duraciones PE.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17900" yWindow="460" windowWidth="10900" windowHeight="16520" tabRatio="500"/>
+    <workbookView xWindow="17900" yWindow="460" windowWidth="10900" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -402,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,7 +640,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -664,7 +664,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -681,7 +681,7 @@
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <f>SUM(A20:A33)</f>
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B34" s="1">
         <f>SUM(B20:B33)</f>
@@ -905,7 +905,7 @@
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
         <f>SUM(A18,A34,A41,A51,A59)</f>
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="B62">
         <f>SUM(B18,B34,B41,B51,B59)</f>

</xml_diff>

<commit_message>
Finalizado completamente Análisis. Realizada la revisión del documento.
</commit_message>
<xml_diff>
--- a/Cálculo duraciones PE.xlsx
+++ b/Cálculo duraciones PE.xlsx
@@ -656,7 +656,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B31">
         <v>2</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -681,7 +681,7 @@
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <f>SUM(A20:A33)</f>
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B34" s="1">
         <f>SUM(B20:B33)</f>
@@ -905,7 +905,7 @@
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
         <f>SUM(A18,A34,A41,A51,A59)</f>
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B62">
         <f>SUM(B18,B34,B41,B51,B59)</f>

</xml_diff>

<commit_message>
Proyecto en Netbeans. Hecho el filechooser.
</commit_message>
<xml_diff>
--- a/Cálculo duraciones PE.xlsx
+++ b/Cálculo duraciones PE.xlsx
@@ -402,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -746,7 +746,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B42">
         <v>12</v>
@@ -755,7 +755,7 @@
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <f>SUM(A36:A42)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B43" s="1">
         <f>SUM(B36:B42)</f>
@@ -921,7 +921,7 @@
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64">
         <f>SUM(A18,A34,A43,A53,A61)</f>
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B64">
         <f>SUM(B18,B34,B43,B53,B61)</f>

</xml_diff>

<commit_message>
Ya abre los archivos: STP, STL, PLY, WRL, OBJ
</commit_message>
<xml_diff>
--- a/Cálculo duraciones PE.xlsx
+++ b/Cálculo duraciones PE.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -16,6 +16,9 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -402,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -722,7 +725,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B39">
         <v>5</v>
@@ -730,15 +733,15 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -746,41 +749,41 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>12</v>
+      </c>
+      <c r="B43">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <f>SUM(A36:A43)</f>
+        <v>136</v>
+      </c>
+      <c r="B44" s="1">
+        <f>SUM(B36:B43)</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="26" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B42">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
-        <f>SUM(A36:A42)</f>
-        <v>15</v>
-      </c>
-      <c r="B43" s="1">
-        <f>SUM(B36:B42)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="26" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>0</v>
-      </c>
-      <c r="B45">
-        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B46">
         <v>5</v>
@@ -788,7 +791,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B47">
         <v>5</v>
@@ -799,15 +802,15 @@
         <v>0</v>
       </c>
       <c r="B48">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B49">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -828,7 +831,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B52">
         <v>28</v>
@@ -836,12 +839,12 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <f>SUM(A45:A52)</f>
-        <v>0</v>
+        <f>SUM(A46:A52)</f>
+        <v>17</v>
       </c>
       <c r="B53" s="1">
-        <f>SUM(B45:B52)</f>
-        <v>58</v>
+        <f>SUM(B46:B52)</f>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="26" x14ac:dyDescent="0.3">
@@ -920,12 +923,12 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64">
-        <f>SUM(A18,A34,A43,A53,A61)</f>
-        <v>93</v>
+        <f>SUM(A18,A34,A44,A53,A61)</f>
+        <v>231</v>
       </c>
       <c r="B64">
-        <f>SUM(B18,B34,B43,B53,B61)</f>
-        <v>207</v>
+        <f>SUM(B18,B34,B44,B53,B61)</f>
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>